<commit_message>
fix bug, check duplicate edu name
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc-loi.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc-loi.xlsx
@@ -119,13 +119,13 @@
     <t>HE130576</t>
   </si>
   <si>
-    <t>Phạm Thanh Hà</t>
-  </si>
-  <si>
     <t>Lừa trái tim đàn bà</t>
   </si>
   <si>
     <t>Tình một đêm</t>
+  </si>
+  <si>
+    <t>Phạm Thanh Hà0</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -559,7 +559,7 @@
         <v>7.5</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -620,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
fix bug display error when import excel
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc-loi.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc-loi.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BachHV\Desktop\New folder (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD1AACC-1527-49EC-9105-083FC3633E27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -108,6 +107,9 @@
     <t>23/07/1999</t>
   </si>
   <si>
+    <t>Sáo</t>
+  </si>
+  <si>
     <t>ĐTR101</t>
   </si>
   <si>
@@ -117,35 +119,23 @@
     <t>HE130576</t>
   </si>
   <si>
-    <t>Phạm Thanh Hà</t>
-  </si>
-  <si>
-    <t>HE 130576</t>
-  </si>
-  <si>
-    <t>HE 130576@%</t>
-  </si>
-  <si>
-    <t>Sáo 21</t>
-  </si>
-  <si>
-    <t>Lừa trái tim đàn bà @$</t>
+    <t>Lừa trái tim đàn bà</t>
+  </si>
+  <si>
+    <t>Tình một đêm</t>
+  </si>
+  <si>
+    <t>Phạm Thanh Hà0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -452,11 +442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,10 +506,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -529,9 +519,6 @@
       </c>
       <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -553,12 +540,6 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
       <c r="D3" t="s">
         <v>25</v>
       </c>
@@ -571,14 +552,14 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
       <c r="J3">
         <v>7.5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -588,12 +569,6 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" t="s">
         <v>26</v>
       </c>
@@ -606,9 +581,6 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
@@ -616,7 +588,7 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -627,9 +599,6 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
         <v>30</v>
       </c>
       <c r="D5" t="s">
@@ -641,27 +610,23 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>